<commit_message>
config and program updates
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Code\hmi-data-merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2F99C1-5F8C-4525-9A1C-818344989FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F207E9-5CBE-4D4A-B1C0-BFF31426B7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="630" windowWidth="23640" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="630" windowWidth="23640" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PyToolConfig" sheetId="1" r:id="rId1"/>
+    <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1318,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD8723F-4287-4CB2-995D-6CC3DAD418FD}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>